<commit_message>
Trial 22 finished. Added trial 22 data to slope evaluation.
</commit_message>
<xml_diff>
--- a/tests/SlopeEvaluation.xlsx
+++ b/tests/SlopeEvaluation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\PrivateNoBackup\git\TX16S_HallDriftComp\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A131345F-F024-470C-82C1-35152B8FF2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A992F854-520F-4EE7-A734-2D6C84A247EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{638E81DC-150D-4F36-BBDF-B4A91D40832C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{638E81DC-150D-4F36-BBDF-B4A91D40832C}"/>
   </bookViews>
   <sheets>
     <sheet name="SlopeAnalysis" sheetId="1" r:id="rId1"/>
+    <sheet name="TempDependance" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>ADC at 20°C</t>
   </si>
@@ -70,6 +71,9 @@
   </si>
   <si>
     <t>ambient center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -600 digits</t>
   </si>
 </sst>
 </file>
@@ -357,6 +361,9 @@
                 <c:pt idx="6">
                   <c:v>1035</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>953</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -387,13 +394,16 @@
                 <c:pt idx="6">
                   <c:v>9.2100000000000001E-2</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1638</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F667-40DF-96F0-4C533A149306}"/>
+              <c16:uniqueId val="{00000000-96B9-45E3-A507-4E3D190C4D09}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -454,6 +464,9 @@
                 <c:pt idx="6">
                   <c:v>1020</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>938</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -484,13 +497,16 @@
                 <c:pt idx="6">
                   <c:v>-4.7899999999999998E-2</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F667-40DF-96F0-4C533A149306}"/>
+              <c16:uniqueId val="{00000001-96B9-45E3-A507-4E3D190C4D09}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -510,7 +526,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200"/>
-          <c:min val="1000"/>
+          <c:min val="900"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -823,11 +839,6 @@
       <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1387,31 +1398,34 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BCF4DC27-827B-4546-A096-50E5047B4244}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>147636</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9300253" cy="6014663"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8952865-802F-4655-9627-10540D44F9E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3D27E22-21EC-46B2-9A56-B9254D32665F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1424,7 +1438,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1725,9 +1739,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CBA376-C6C8-4A8C-AE9A-3FF9B48D44AA}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -1887,6 +1901,23 @@
         <v>-4.7899999999999998E-2</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2">
+        <v>953</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.1638</v>
+      </c>
+      <c r="D10" s="2">
+        <v>938</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.21</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
@@ -1895,6 +1926,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>